<commit_message>
Added Configurable zero_before_threshold parameter to enable setting dims before noise_threshold or First Rise Point to 0
</commit_message>
<xml_diff>
--- a/on_trucks/Processed_Stand_Alone/10_245-70R19.xlsx
+++ b/on_trucks/Processed_Stand_Alone/10_245-70R19.xlsx
@@ -10567,19 +10567,19 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>128</v>
       </c>
       <c r="E2">
-        <v>0.008633308113208046</v>
+        <v>0.008441812073723569</v>
       </c>
       <c r="F2">
         <v>0.5179725647211256</v>
       </c>
       <c r="G2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -10608,19 +10608,19 @@
         <v>0.5</v>
       </c>
       <c r="C3">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>130</v>
       </c>
       <c r="E3">
-        <v>0.004730630713836136</v>
+        <v>0.004705503334542409</v>
       </c>
       <c r="F3">
         <v>0.5569833561621805</v>
       </c>
       <c r="G3">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -10649,19 +10649,19 @@
         <v>0.5</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>130</v>
       </c>
       <c r="E4">
-        <v>0.005479873671755744</v>
+        <v>0.005337774033308033</v>
       </c>
       <c r="F4">
         <v>0.550765826740669</v>
       </c>
       <c r="G4">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -10690,19 +10690,19 @@
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>130</v>
       </c>
       <c r="E5">
-        <v>0.00602823942627983</v>
+        <v>0.006026037585510682</v>
       </c>
       <c r="F5">
         <v>0.5321082614000309</v>
       </c>
       <c r="G5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -10731,19 +10731,19 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>129</v>
       </c>
       <c r="E6">
-        <v>0.006317664092323982</v>
+        <v>0.005940632590531252</v>
       </c>
       <c r="F6">
         <v>0.5128866026012472</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -10826,19 +10826,19 @@
         <v>0.7</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>140</v>
       </c>
       <c r="E2">
-        <v>0.008633308113208046</v>
+        <v>0.008441812073723569</v>
       </c>
       <c r="F2">
         <v>0.7231067219592636</v>
       </c>
       <c r="G2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -10867,19 +10867,19 @@
         <v>0.7</v>
       </c>
       <c r="C3">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>140</v>
       </c>
       <c r="E3">
-        <v>0.004730630713836136</v>
+        <v>0.004705503334542409</v>
       </c>
       <c r="F3">
         <v>0.720212790804176</v>
       </c>
       <c r="G3">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -10908,19 +10908,19 @@
         <v>0.7</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>141</v>
       </c>
       <c r="E4">
-        <v>0.005479873671755744</v>
+        <v>0.005337774033308033</v>
       </c>
       <c r="F4">
         <v>0.7034637045612355</v>
       </c>
       <c r="G4">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -10949,19 +10949,19 @@
         <v>0.7</v>
       </c>
       <c r="C5">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>140</v>
       </c>
       <c r="E5">
-        <v>0.00602823942627983</v>
+        <v>0.006026037585510682</v>
       </c>
       <c r="F5">
         <v>0.7095630021689322</v>
       </c>
       <c r="G5">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -10990,19 +10990,19 @@
         <v>0.7</v>
       </c>
       <c r="C6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>139</v>
       </c>
       <c r="E6">
-        <v>0.006317664092323982</v>
+        <v>0.005940632590531252</v>
       </c>
       <c r="F6">
         <v>0.7013986153637926</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -11085,19 +11085,19 @@
         <v>0.8</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>149</v>
       </c>
       <c r="E2">
-        <v>0.008633308113208046</v>
+        <v>0.008441812073723569</v>
       </c>
       <c r="F2">
         <v>0.8099808876985989</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -11126,19 +11126,19 @@
         <v>0.8</v>
       </c>
       <c r="C3">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>150</v>
       </c>
       <c r="E3">
-        <v>0.004730630713836136</v>
+        <v>0.004705503334542409</v>
       </c>
       <c r="F3">
         <v>0.8076400705167959</v>
       </c>
       <c r="G3">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -11167,19 +11167,19 @@
         <v>0.8</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>150</v>
       </c>
       <c r="E4">
-        <v>0.005479873671755744</v>
+        <v>0.005337774033308033</v>
       </c>
       <c r="F4">
         <v>0.8112933141246061</v>
       </c>
       <c r="G4">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -11208,19 +11208,19 @@
         <v>0.8</v>
       </c>
       <c r="C5">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="E5">
-        <v>0.00602823942627983</v>
+        <v>0.006026037585510682</v>
       </c>
       <c r="F5">
         <v>0.8071372237932151</v>
       </c>
       <c r="G5">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -11249,19 +11249,19 @@
         <v>0.8</v>
       </c>
       <c r="C6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>149</v>
       </c>
       <c r="E6">
-        <v>0.006317664092323982</v>
+        <v>0.005940632590531252</v>
       </c>
       <c r="F6">
         <v>0.8092446710557867</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -11344,19 +11344,19 @@
         <v>0.9</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>164</v>
       </c>
       <c r="E2">
-        <v>0.008633308113208046</v>
+        <v>0.008441812073723569</v>
       </c>
       <c r="F2">
         <v>0.9023100645601745</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -11385,19 +11385,19 @@
         <v>0.9</v>
       </c>
       <c r="C3">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>165</v>
       </c>
       <c r="E3">
-        <v>0.004730630713836136</v>
+        <v>0.004705503334542409</v>
       </c>
       <c r="F3">
         <v>0.9049918317004615</v>
       </c>
       <c r="G3">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -11426,19 +11426,19 @@
         <v>0.9</v>
       </c>
       <c r="C4">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>164</v>
       </c>
       <c r="E4">
-        <v>0.005479873671755744</v>
+        <v>0.005337774033308033</v>
       </c>
       <c r="F4">
         <v>0.9000839259122227</v>
       </c>
       <c r="G4">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -11467,19 +11467,19 @@
         <v>0.9</v>
       </c>
       <c r="C5">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>165</v>
       </c>
       <c r="E5">
-        <v>0.00602823942627983</v>
+        <v>0.006026037585510682</v>
       </c>
       <c r="F5">
         <v>0.9028302784984203</v>
       </c>
       <c r="G5">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -11508,19 +11508,19 @@
         <v>0.9</v>
       </c>
       <c r="C6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>164</v>
       </c>
       <c r="E6">
-        <v>0.006317664092323982</v>
+        <v>0.005940632590531252</v>
       </c>
       <c r="F6">
         <v>0.9189516736979139</v>
       </c>
       <c r="G6">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H6">
         <v>10</v>

</xml_diff>

<commit_message>
Added Tire Type Filtering for dashboard script and cleanup of Tire Type extraction in process_audio_to_csv script
</commit_message>
<xml_diff>
--- a/on_trucks/Processed_Stand_Alone/10_245-70R19.xlsx
+++ b/on_trucks/Processed_Stand_Alone/10_245-70R19.xlsx
@@ -677,13 +677,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.2377663101126416</v>
+        <v>0.1883562720413256</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.02510516389178956</v>
       </c>
       <c r="G2">
-        <v>0.3723824370219362</v>
+        <v>0.2806140951908258</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -692,22 +692,22 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.01799627644658349</v>
       </c>
       <c r="K2">
-        <v>0.09700642977460434</v>
+        <v>0.09188788860966107</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>0.01772962084126473</v>
       </c>
       <c r="N2">
-        <v>0.08916778570127046</v>
+        <v>0.08651575188835429</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.007515628400145689</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -716,31 +716,31 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0.06203645274374392</v>
+        <v>0.0679215628021367</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>0.009354707817189264</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>0.009409078027060314</v>
       </c>
       <c r="U2">
-        <v>0.05412130604056362</v>
+        <v>0.06249699576466432</v>
       </c>
       <c r="V2">
         <v>0</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>0.0009130098233818617</v>
       </c>
       <c r="X2">
-        <v>0.0875192786052397</v>
+        <v>0.08538596395270243</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>0.01451133998321967</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>0.02045269134469629</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>0.0138339531749992</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -787,13 +787,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.3457160286146471</v>
+        <v>0.2810718858277978</v>
       </c>
       <c r="F3">
-        <v>0.09556791649791392</v>
+        <v>0.09570109906500639</v>
       </c>
       <c r="G3">
-        <v>0.3823040290291285</v>
+        <v>0.3081852082731207</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -802,19 +802,19 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.0043345091647187</v>
       </c>
       <c r="K3">
-        <v>0.1212261277871134</v>
+        <v>0.1147149655833565</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.00793617876372193</v>
       </c>
       <c r="M3">
-        <v>0.002260934458020116</v>
+        <v>0.02655650898660795</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.01184477026260017</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -823,19 +823,19 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>0.002125668525927968</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.007929201533682935</v>
       </c>
       <c r="S3">
-        <v>0.0008071050288407967</v>
+        <v>0.02547915724157416</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>0.01472853565955751</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -844,13 +844,13 @@
         <v>0</v>
       </c>
       <c r="X3">
-        <v>0.05211785858433611</v>
+        <v>0.06350268928220477</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>0.005367150936926981</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -877,10 +877,10 @@
         <v>0</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>0.008915787724415331</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>0.02160668316878013</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -897,13 +897,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.3366986924867602</v>
+        <v>0.2847639121176406</v>
       </c>
       <c r="F4">
-        <v>0.1503091983582091</v>
+        <v>0.1407597575663971</v>
       </c>
       <c r="G4">
-        <v>0.3187772531855677</v>
+        <v>0.2709178435558056</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -915,16 +915,16 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0.1283580054213029</v>
+        <v>0.1238003093150366</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.01895901933885585</v>
       </c>
       <c r="M4">
-        <v>0.009248231602647625</v>
+        <v>0.03177633361973534</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.004106824489686503</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -933,19 +933,19 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>0.003039826768261577</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>0.01598442663664308</v>
       </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>0.004849594737302712</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <v>0.05660861894551232</v>
+        <v>0.06836687521874248</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -984,13 +984,13 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>0</v>
+        <v>0.000849403767639064</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>0.01497005020782152</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>0.01685582266043188</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -1007,34 +1007,34 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.2659020674170398</v>
+        <v>0.2016516135182773</v>
       </c>
       <c r="F5">
-        <v>0.0227304343382684</v>
+        <v>0.04034648798539808</v>
       </c>
       <c r="G5">
-        <v>0.4494081650546196</v>
+        <v>0.3233782875579669</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.007408307741336323</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.009735064150875309</v>
+        <v>0.03172615759207197</v>
       </c>
       <c r="K5">
-        <v>0.1240314029742299</v>
+        <v>0.1075433285689083</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>0.01045456113914201</v>
       </c>
       <c r="M5">
-        <v>0.01200690470975754</v>
+        <v>0.03323315708005286</v>
       </c>
       <c r="N5">
-        <v>0.0003081130030836854</v>
+        <v>0.02547289721365328</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1046,16 +1046,16 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>0.02467773573741563</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>0.01150139106056939</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0.01493207102936305</v>
+        <v>0.03517353274975801</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1064,13 +1064,13 @@
         <v>0</v>
       </c>
       <c r="X5">
-        <v>0.1009457773227627</v>
+        <v>0.09222974245457435</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>0.01130436783930669</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>0.02186882985574325</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1097,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>0.003305170023756752</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>0.01872443188206918</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -1114,16 +1114,16 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.005630125271338065</v>
       </c>
       <c r="E6">
-        <v>0.2504593990864346</v>
+        <v>0.2212141198256587</v>
       </c>
       <c r="F6">
-        <v>0.2572375251510468</v>
+        <v>0.2265284776502698</v>
       </c>
       <c r="G6">
-        <v>0.1988439662844848</v>
+        <v>0.1807452827802943</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1132,16 +1132,16 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.005106432762393669</v>
       </c>
       <c r="K6">
-        <v>0.2199697496996367</v>
+        <v>0.1973088537913883</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.01555486107933129</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>0.003096913791262934</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1153,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>0.009917407698003351</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>0.01354812936084224</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1171,10 +1171,10 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>0.01871049013293005</v>
       </c>
       <c r="X6">
-        <v>0.07348935977839705</v>
+        <v>0.0824615938098706</v>
       </c>
       <c r="Y6">
         <v>0</v>
@@ -1204,10 +1204,10 @@
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>0</v>
+        <v>0.002053884637459715</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>0.01812342740895694</v>
       </c>
       <c r="AJ6">
         <v>0</v>
@@ -1350,97 +1350,97 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.2377663101126416</v>
+        <v>0.1883562720413256</v>
       </c>
       <c r="F2">
-        <v>0.2377663101126416</v>
+        <v>0.2134614359331152</v>
       </c>
       <c r="G2">
-        <v>0.6101487471345779</v>
+        <v>0.4940755311239409</v>
       </c>
       <c r="H2">
-        <v>0.6101487471345779</v>
+        <v>0.4940755311239409</v>
       </c>
       <c r="I2">
-        <v>0.6101487471345779</v>
+        <v>0.4940755311239409</v>
       </c>
       <c r="J2">
-        <v>0.6101487471345779</v>
+        <v>0.5120718075705244</v>
       </c>
       <c r="K2">
-        <v>0.7071551769091823</v>
+        <v>0.6039596961801854</v>
       </c>
       <c r="L2">
-        <v>0.7071551769091823</v>
+        <v>0.6039596961801854</v>
       </c>
       <c r="M2">
-        <v>0.7071551769091823</v>
+        <v>0.6216893170214501</v>
       </c>
       <c r="N2">
-        <v>0.7963229626104528</v>
+        <v>0.7082050689098044</v>
       </c>
       <c r="O2">
-        <v>0.7963229626104528</v>
+        <v>0.71572069730995</v>
       </c>
       <c r="P2">
-        <v>0.7963229626104528</v>
+        <v>0.71572069730995</v>
       </c>
       <c r="Q2">
-        <v>0.7963229626104528</v>
+        <v>0.71572069730995</v>
       </c>
       <c r="R2">
-        <v>0.8583594153541967</v>
+        <v>0.7836422601120867</v>
       </c>
       <c r="S2">
-        <v>0.8583594153541967</v>
+        <v>0.792996967929276</v>
       </c>
       <c r="T2">
-        <v>0.8583594153541967</v>
+        <v>0.8024060459563362</v>
       </c>
       <c r="U2">
-        <v>0.9124807213947603</v>
+        <v>0.8649030417210005</v>
       </c>
       <c r="V2">
-        <v>0.9124807213947603</v>
+        <v>0.8649030417210005</v>
       </c>
       <c r="W2">
-        <v>0.9124807213947603</v>
+        <v>0.8658160515443823</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0.9512020154970848</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>0.9657133554803045</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AB2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AE2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AI2">
-        <v>1</v>
+        <v>0.9861660468250008</v>
       </c>
       <c r="AJ2">
         <v>1</v>
@@ -1460,97 +1460,97 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.3457160286146471</v>
+        <v>0.2810718858277978</v>
       </c>
       <c r="F3">
-        <v>0.441283945112561</v>
+        <v>0.3767729848928042</v>
       </c>
       <c r="G3">
-        <v>0.8235879741416895</v>
+        <v>0.6849581931659249</v>
       </c>
       <c r="H3">
-        <v>0.8235879741416895</v>
+        <v>0.6849581931659249</v>
       </c>
       <c r="I3">
-        <v>0.8235879741416895</v>
+        <v>0.6849581931659249</v>
       </c>
       <c r="J3">
-        <v>0.8235879741416895</v>
+        <v>0.6892927023306435</v>
       </c>
       <c r="K3">
-        <v>0.944814101928803</v>
+        <v>0.8040076679140001</v>
       </c>
       <c r="L3">
-        <v>0.944814101928803</v>
+        <v>0.811943846677722</v>
       </c>
       <c r="M3">
-        <v>0.9470750363868231</v>
+        <v>0.83850035566433</v>
       </c>
       <c r="N3">
-        <v>0.9470750363868231</v>
+        <v>0.8503451259269302</v>
       </c>
       <c r="O3">
-        <v>0.9470750363868231</v>
+        <v>0.8503451259269302</v>
       </c>
       <c r="P3">
-        <v>0.9470750363868231</v>
+        <v>0.8503451259269302</v>
       </c>
       <c r="Q3">
-        <v>0.9470750363868231</v>
+        <v>0.8524707944528582</v>
       </c>
       <c r="R3">
-        <v>0.9470750363868231</v>
+        <v>0.8603999959865412</v>
       </c>
       <c r="S3">
-        <v>0.947882141415664</v>
+        <v>0.8858791532281153</v>
       </c>
       <c r="T3">
-        <v>0.947882141415664</v>
+        <v>0.8858791532281153</v>
       </c>
       <c r="U3">
-        <v>0.947882141415664</v>
+        <v>0.9006076888876728</v>
       </c>
       <c r="V3">
-        <v>0.947882141415664</v>
+        <v>0.9006076888876728</v>
       </c>
       <c r="W3">
-        <v>0.947882141415664</v>
+        <v>0.9006076888876728</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>0.9641103781698777</v>
       </c>
       <c r="Y3">
-        <v>1</v>
+        <v>0.9641103781698777</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AB3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AC3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AD3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AE3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AF3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AG3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AH3">
-        <v>1</v>
+        <v>0.9694775291068046</v>
       </c>
       <c r="AI3">
-        <v>1</v>
+        <v>0.97839331683122</v>
       </c>
       <c r="AJ3">
         <v>1</v>
@@ -1570,97 +1570,97 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.3366986924867602</v>
+        <v>0.2847639121176406</v>
       </c>
       <c r="F4">
-        <v>0.4870078908449693</v>
+        <v>0.4255236696840377</v>
       </c>
       <c r="G4">
-        <v>0.805785144030537</v>
+        <v>0.6964415132398433</v>
       </c>
       <c r="H4">
-        <v>0.805785144030537</v>
+        <v>0.6964415132398433</v>
       </c>
       <c r="I4">
-        <v>0.805785144030537</v>
+        <v>0.6964415132398433</v>
       </c>
       <c r="J4">
-        <v>0.805785144030537</v>
+        <v>0.6964415132398433</v>
       </c>
       <c r="K4">
-        <v>0.93414314945184</v>
+        <v>0.8202418225548799</v>
       </c>
       <c r="L4">
-        <v>0.93414314945184</v>
+        <v>0.8392008418937358</v>
       </c>
       <c r="M4">
-        <v>0.9433913810544876</v>
+        <v>0.8709771755134711</v>
       </c>
       <c r="N4">
-        <v>0.9433913810544876</v>
+        <v>0.8750840000031576</v>
       </c>
       <c r="O4">
-        <v>0.9433913810544876</v>
+        <v>0.8750840000031576</v>
       </c>
       <c r="P4">
-        <v>0.9433913810544876</v>
+        <v>0.8750840000031576</v>
       </c>
       <c r="Q4">
-        <v>0.9433913810544876</v>
+        <v>0.8781238267714191</v>
       </c>
       <c r="R4">
-        <v>0.9433913810544876</v>
+        <v>0.8781238267714191</v>
       </c>
       <c r="S4">
-        <v>0.9433913810544876</v>
+        <v>0.8941082534080622</v>
       </c>
       <c r="T4">
-        <v>0.9433913810544876</v>
+        <v>0.8941082534080622</v>
       </c>
       <c r="U4">
-        <v>0.9433913810544876</v>
+        <v>0.8989578481453649</v>
       </c>
       <c r="V4">
-        <v>0.9433913810544876</v>
+        <v>0.8989578481453649</v>
       </c>
       <c r="W4">
-        <v>0.9433913810544876</v>
+        <v>0.8989578481453649</v>
       </c>
       <c r="X4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="Y4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="Z4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AA4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AB4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AC4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AD4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AE4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AF4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AG4">
-        <v>0.9999999999999999</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="AH4">
-        <v>0.9999999999999999</v>
+        <v>0.9681741271317466</v>
       </c>
       <c r="AI4">
-        <v>0.9999999999999999</v>
+        <v>0.983144177339568</v>
       </c>
       <c r="AJ4">
         <v>0.9999999999999999</v>
@@ -1680,100 +1680,100 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.2659020674170398</v>
+        <v>0.2016516135182773</v>
       </c>
       <c r="F5">
-        <v>0.2886325017553081</v>
+        <v>0.2419981015036753</v>
       </c>
       <c r="G5">
-        <v>0.7380406668099277</v>
+        <v>0.5653763890616422</v>
       </c>
       <c r="H5">
-        <v>0.7380406668099277</v>
+        <v>0.5727846968029785</v>
       </c>
       <c r="I5">
-        <v>0.7380406668099277</v>
+        <v>0.5727846968029785</v>
       </c>
       <c r="J5">
-        <v>0.7477757309608031</v>
+        <v>0.6045108543950505</v>
       </c>
       <c r="K5">
-        <v>0.8718071339350331</v>
+        <v>0.7120541829639587</v>
       </c>
       <c r="L5">
-        <v>0.8718071339350331</v>
+        <v>0.7225087441031007</v>
       </c>
       <c r="M5">
-        <v>0.8838140386447906</v>
+        <v>0.7557419011831535</v>
       </c>
       <c r="N5">
-        <v>0.8841221516478742</v>
+        <v>0.7812147983968069</v>
       </c>
       <c r="O5">
-        <v>0.8841221516478742</v>
+        <v>0.7812147983968069</v>
       </c>
       <c r="P5">
-        <v>0.8841221516478742</v>
+        <v>0.7812147983968069</v>
       </c>
       <c r="Q5">
-        <v>0.8841221516478742</v>
+        <v>0.7812147983968069</v>
       </c>
       <c r="R5">
-        <v>0.8841221516478742</v>
+        <v>0.8058925341342225</v>
       </c>
       <c r="S5">
-        <v>0.8841221516478742</v>
+        <v>0.8173939251947918</v>
       </c>
       <c r="T5">
-        <v>0.8841221516478742</v>
+        <v>0.8173939251947918</v>
       </c>
       <c r="U5">
-        <v>0.8990542226772372</v>
+        <v>0.8525674579445498</v>
       </c>
       <c r="V5">
-        <v>0.8990542226772372</v>
+        <v>0.8525674579445498</v>
       </c>
       <c r="W5">
-        <v>0.8990542226772372</v>
+        <v>0.8525674579445498</v>
       </c>
       <c r="X5">
-        <v>0.9999999999999999</v>
+        <v>0.9447972003991242</v>
       </c>
       <c r="Y5">
-        <v>0.9999999999999999</v>
+        <v>0.9561015682384308</v>
       </c>
       <c r="Z5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AA5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AB5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AC5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AD5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AE5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AF5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AG5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AH5">
-        <v>0.9999999999999999</v>
+        <v>0.9779703980941741</v>
       </c>
       <c r="AI5">
-        <v>0.9999999999999999</v>
+        <v>0.9812755681179308</v>
       </c>
       <c r="AJ5">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -1787,103 +1787,103 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.005630125271338065</v>
       </c>
       <c r="E6">
-        <v>0.2504593990864346</v>
+        <v>0.2268442450969968</v>
       </c>
       <c r="F6">
-        <v>0.5076969242374814</v>
+        <v>0.4533727227472666</v>
       </c>
       <c r="G6">
-        <v>0.7065408905219661</v>
+        <v>0.6341180055275609</v>
       </c>
       <c r="H6">
-        <v>0.7065408905219661</v>
+        <v>0.6341180055275609</v>
       </c>
       <c r="I6">
-        <v>0.7065408905219661</v>
+        <v>0.6341180055275609</v>
       </c>
       <c r="J6">
-        <v>0.7065408905219661</v>
+        <v>0.6392244382899546</v>
       </c>
       <c r="K6">
-        <v>0.9265106402216028</v>
+        <v>0.8365332920813429</v>
       </c>
       <c r="L6">
-        <v>0.9265106402216028</v>
+        <v>0.8520881531606741</v>
       </c>
       <c r="M6">
-        <v>0.9265106402216028</v>
+        <v>0.8551850669519371</v>
       </c>
       <c r="N6">
-        <v>0.9265106402216028</v>
+        <v>0.8551850669519371</v>
       </c>
       <c r="O6">
-        <v>0.9265106402216028</v>
+        <v>0.8551850669519371</v>
       </c>
       <c r="P6">
-        <v>0.9265106402216028</v>
+        <v>0.8551850669519371</v>
       </c>
       <c r="Q6">
-        <v>0.9265106402216028</v>
+        <v>0.8651024746499404</v>
       </c>
       <c r="R6">
-        <v>0.9265106402216028</v>
+        <v>0.8651024746499404</v>
       </c>
       <c r="S6">
-        <v>0.9265106402216028</v>
+        <v>0.8651024746499404</v>
       </c>
       <c r="T6">
-        <v>0.9265106402216028</v>
+        <v>0.8786506040107827</v>
       </c>
       <c r="U6">
-        <v>0.9265106402216028</v>
+        <v>0.8786506040107827</v>
       </c>
       <c r="V6">
-        <v>0.9265106402216028</v>
+        <v>0.8786506040107827</v>
       </c>
       <c r="W6">
-        <v>0.9265106402216028</v>
+        <v>0.8973610941437127</v>
       </c>
       <c r="X6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="Y6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="Z6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AA6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AB6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AC6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AD6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AE6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AF6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AG6">
-        <v>0.9999999999999998</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="AH6">
-        <v>0.9999999999999998</v>
+        <v>0.981876572591043</v>
       </c>
       <c r="AI6">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="AJ6">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1951,16 +1951,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.6101487471345779</v>
+        <v>0.5120718075705244</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8235879741416895</v>
+        <v>0.6849581931659249</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -2039,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.805785144030537</v>
+        <v>0.6964415132398433</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -2080,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.7380406668099277</v>
+        <v>0.5653763890616422</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2115,16 +2115,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.5076969242374814</v>
+        <v>0.6341180055275609</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -2210,16 +2210,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.7071551769091823</v>
+        <v>0.7082050689098044</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -2251,16 +2251,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8235879741416895</v>
+        <v>0.8040076679140001</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2292,16 +2292,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.805785144030537</v>
+        <v>0.8202418225548799</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2333,16 +2333,16 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.7380406668099277</v>
+        <v>0.7120541829639587</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -2374,16 +2374,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.7065408905219661</v>
+        <v>0.8365332920813429</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -2469,16 +2469,16 @@
         <v>2</v>
       </c>
       <c r="D2">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.8024060459563362</v>
+      </c>
+      <c r="G2">
         <v>17</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0.8583594153541967</v>
-      </c>
-      <c r="G2">
-        <v>15</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -2510,16 +2510,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8235879741416895</v>
+        <v>0.8040076679140001</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2551,16 +2551,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.805785144030537</v>
+        <v>0.8202418225548799</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2592,16 +2592,16 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8718071339350331</v>
+        <v>0.8058925341342225</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.9265106402216028</v>
+        <v>0.8365332920813429</v>
       </c>
       <c r="G6">
         <v>8</v>
@@ -2728,16 +2728,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.9124807213947603</v>
+        <v>0.9512020154970848</v>
       </c>
       <c r="G2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -2769,16 +2769,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.944814101928803</v>
+        <v>0.9006076888876728</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2810,16 +2810,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.93414314945184</v>
+        <v>0.9673247233641075</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.9999999999999999</v>
+        <v>0.9447972003991242</v>
       </c>
       <c r="G5">
         <v>21</v>
@@ -2892,16 +2892,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.9265106402216028</v>
+        <v>0.9798226879535833</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H6">
         <v>10</v>

</xml_diff>